<commit_message>
Fixed errors in excel file
</commit_message>
<xml_diff>
--- a/Software/DeepLearning/SpeedTests/Plotting/SpeedTestWithNUC.xlsx
+++ b/Software/DeepLearning/SpeedTests/Plotting/SpeedTestWithNUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\prg_prgeye\Software\DeepLearning\SpeedTests\Plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7542499-9C49-4DBC-9255-C82C6B772AE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDDBE9E-623C-4191-9B7B-06749C546C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -897,8 +897,8 @@
   <dimension ref="A1:Y67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K23" sqref="K23"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -914,7 +914,8 @@
     <col min="9" max="9" width="8" customWidth="1"/>
     <col min="10" max="10" width="11.46484375" customWidth="1"/>
     <col min="11" max="11" width="18.3984375" customWidth="1"/>
-    <col min="12" max="14" width="16.1328125" customWidth="1"/>
+    <col min="12" max="13" width="16.1328125" customWidth="1"/>
+    <col min="14" max="14" width="12.59765625" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
     <col min="16" max="16" width="7.73046875" customWidth="1"/>
     <col min="17" max="17" width="6.86328125" customWidth="1"/>
@@ -1326,7 +1327,7 @@
         <v>566.71895668575803</v>
       </c>
       <c r="O7" s="41">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="P7" s="42">
         <v>367207931</v>
@@ -1344,21 +1345,21 @@
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>3.9522722712374295E-2</v>
+        <v>4.0854949320656579E-2</v>
       </c>
       <c r="U7" s="33">
         <f t="shared" si="3"/>
-        <v>0.22235733287249995</v>
+        <v>0.22985252386820221</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
-        <v>81.651376146788991</v>
+        <v>84.403669724770651</v>
       </c>
       <c r="W7" s="21"/>
       <c r="X7" s="21"/>
       <c r="Y7">
         <f>H7*V7/1000</f>
-        <v>10.100866701331523</v>
+        <v>10.441345354185396</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1405,7 +1406,7 @@
         <v>1.9963773850387401</v>
       </c>
       <c r="O8" s="41">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="P8" s="42">
         <v>367207931</v>
@@ -1423,20 +1424,20 @@
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>3.9522722712374295E-2</v>
+        <v>4.0854949320656579E-2</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>0.22235733287249995</v>
+        <v>0.22985252386820221</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
-        <v>81.651376146788991</v>
+        <v>84.403669724770651</v>
       </c>
       <c r="W8" s="21"/>
       <c r="X8">
         <f>C8*V8/1000</f>
-        <v>1.5726055045871561</v>
+        <v>1.6256146788990828</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1479,7 +1480,7 @@
       <c r="M9" s="40"/>
       <c r="N9" s="40"/>
       <c r="O9" s="41">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="P9" s="42">
         <v>367207931</v>
@@ -1497,23 +1498,23 @@
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>3.9078647176280207E-2</v>
+        <v>4.0410873784562484E-2</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>0.21985893587393254</v>
+        <v>0.22735412686963477</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
-        <v>80.733944954128447</v>
+        <v>83.486238532110093</v>
       </c>
       <c r="W9">
         <f>V9*L9/1000</f>
-        <v>10.521355719053512</v>
+        <v>10.88003830038488</v>
       </c>
       <c r="X9">
         <f>C9*V9/1000</f>
-        <v>70.561467889908258</v>
+        <v>72.966972477064218</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1600,7 +1601,7 @@
         <v>798.56824084016796</v>
       </c>
       <c r="O12" s="41">
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="P12" s="42">
         <v>151605682</v>
@@ -1618,21 +1619,21 @@
       </c>
       <c r="T12" s="21">
         <f t="shared" si="2"/>
-        <v>0.4169050086922429</v>
+        <v>0.33986821360780667</v>
       </c>
       <c r="U12">
         <f t="shared" si="3"/>
-        <v>0.55673157240089888</v>
+        <v>0.45385726010942845</v>
       </c>
       <c r="V12" s="32">
         <f t="shared" si="4"/>
-        <v>84.403669724770651</v>
+        <v>68.807339449541288</v>
       </c>
       <c r="W12" s="21"/>
       <c r="X12" s="21"/>
       <c r="Y12">
         <f>H12*V12/1000</f>
-        <v>16.628837605043078</v>
+        <v>13.556117612806858</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -1677,7 +1678,7 @@
         <v>4.74227565969725</v>
       </c>
       <c r="O13" s="41">
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="P13" s="42">
         <v>151605682</v>
@@ -1695,20 +1696,20 @@
       </c>
       <c r="T13">
         <f t="shared" si="2"/>
-        <v>0.4169050086922429</v>
+        <v>0.33986821360780667</v>
       </c>
       <c r="U13">
         <f t="shared" si="3"/>
-        <v>0.55673157240089888</v>
+        <v>0.45385726010942845</v>
       </c>
       <c r="V13">
         <f t="shared" si="4"/>
-        <v>84.403669724770651</v>
+        <v>68.807339449541288</v>
       </c>
       <c r="W13" s="21"/>
       <c r="X13">
         <f>C13*V13/1000</f>
-        <v>3.3736146788990826</v>
+        <v>2.7502293577981654</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -1751,7 +1752,7 @@
       <c r="M14" s="40"/>
       <c r="N14" s="40"/>
       <c r="O14" s="41">
-        <v>1.8</v>
+        <v>3.5</v>
       </c>
       <c r="P14" s="42">
         <v>151605682</v>
@@ -1769,23 +1770,23 @@
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>0.41237343251080544</v>
+        <v>0.33533663742636932</v>
       </c>
       <c r="U14">
         <f t="shared" si="3"/>
-        <v>0.55068014226610651</v>
+        <v>0.44780582997463608</v>
       </c>
       <c r="V14" s="31">
         <f t="shared" si="4"/>
-        <v>83.486238532110093</v>
+        <v>67.889908256880744</v>
       </c>
       <c r="W14">
         <f>V14*L14/1000</f>
-        <v>11.754059686472441</v>
+        <v>9.5582463384501164</v>
       </c>
       <c r="X14" s="32">
         <f>C14*V14/1000</f>
-        <v>92.753211009174308</v>
+        <v>75.425688073394497</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -1876,7 +1877,7 @@
         <v>0.17199011234870931</v>
       </c>
       <c r="V16" s="33">
-        <f t="shared" si="4"/>
+        <f>(1 - (O16/10.9))*100</f>
         <v>88.073394495412856</v>
       </c>
       <c r="Y16">
@@ -2120,7 +2121,7 @@
         <v>932.24986219527295</v>
       </c>
       <c r="O21" s="41">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="P21" s="42">
         <v>80098708</v>
@@ -2138,19 +2139,19 @@
       </c>
       <c r="T21" s="38">
         <f t="shared" si="2"/>
-        <v>0.57031800320803872</v>
+        <v>0.5227915029407022</v>
       </c>
       <c r="U21" s="32">
         <f t="shared" si="3"/>
-        <v>0.96211564590387966</v>
+        <v>0.88193934207855629</v>
       </c>
       <c r="V21">
         <f t="shared" si="4"/>
-        <v>77.064220183486242</v>
+        <v>70.642201834862391</v>
       </c>
       <c r="Y21" s="32">
         <f>H21*V21/1000</f>
-        <v>17.292104806954921</v>
+        <v>15.851096073042012</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -2195,7 +2196,7 @@
         <v>5.0002738387347998</v>
       </c>
       <c r="O22" s="41">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="P22" s="42">
         <v>80098708</v>
@@ -2213,19 +2214,19 @@
       </c>
       <c r="T22">
         <f t="shared" si="2"/>
-        <v>0.57031800320803872</v>
+        <v>0.5227915029407022</v>
       </c>
       <c r="U22">
         <f t="shared" si="3"/>
-        <v>0.96211564590387966</v>
+        <v>0.88193934207855629</v>
       </c>
       <c r="V22">
         <f t="shared" si="4"/>
-        <v>77.064220183486242</v>
+        <v>70.642201834862391</v>
       </c>
       <c r="X22">
         <f>C22*V22/1000</f>
-        <v>2.7519633027522938</v>
+        <v>2.5226330275229363</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -2268,7 +2269,7 @@
       <c r="M23" s="40"/>
       <c r="N23" s="40"/>
       <c r="O23" s="41">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="P23" s="42">
         <v>80098708</v>
@@ -2286,15 +2287,15 @@
       </c>
       <c r="T23">
         <f t="shared" si="2"/>
-        <v>0.56352850316984782</v>
+        <v>0.5227915029407022</v>
       </c>
       <c r="U23">
         <f t="shared" si="3"/>
-        <v>0.95066188821454745</v>
+        <v>0.88193934207855629</v>
       </c>
       <c r="V23">
         <f t="shared" si="4"/>
-        <v>76.146788990825684</v>
+        <v>70.642201834862391</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -2869,7 +2870,7 @@
         <v>494.38045441044</v>
       </c>
       <c r="O34" s="41">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="P34" s="42">
         <v>301015853</v>
@@ -2887,19 +2888,19 @@
       </c>
       <c r="T34">
         <f t="shared" si="2"/>
-        <v>3.0723853726635587E-2</v>
+        <v>3.6067132635615694E-2</v>
       </c>
       <c r="U34">
         <f t="shared" si="3"/>
-        <v>0.21029707127610314</v>
+        <v>0.24687047497629494</v>
       </c>
       <c r="V34">
         <f t="shared" si="4"/>
-        <v>63.302752293577981</v>
+        <v>74.311926605504581</v>
       </c>
       <c r="Y34">
         <f>H34*V34/1000</f>
-        <v>8.5934089874587798</v>
+        <v>10.087914898321175</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -2944,7 +2945,7 @@
         <v>2.4048545873662599</v>
       </c>
       <c r="O35" s="41">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="P35" s="42">
         <v>301015853</v>
@@ -2962,19 +2963,19 @@
       </c>
       <c r="T35">
         <f t="shared" si="2"/>
-        <v>3.0723853726635587E-2</v>
+        <v>3.6067132635615694E-2</v>
       </c>
       <c r="U35">
         <f t="shared" si="3"/>
-        <v>0.21029707127610314</v>
+        <v>0.24687047497629494</v>
       </c>
       <c r="V35">
         <f t="shared" si="4"/>
-        <v>63.302752293577981</v>
+        <v>74.311926605504581</v>
       </c>
       <c r="X35">
         <f>C35*V35/1000</f>
-        <v>1.3736697247706422</v>
+        <v>1.6125688073394495</v>
       </c>
     </row>
     <row r="36" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -3017,7 +3018,7 @@
       <c r="M36" s="40"/>
       <c r="N36" s="40"/>
       <c r="O36" s="41">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="P36" s="42">
         <v>301015853</v>
@@ -3035,23 +3036,23 @@
       </c>
       <c r="T36">
         <f t="shared" si="2"/>
-        <v>2.9833307241805572E-2</v>
+        <v>3.5176586150785664E-2</v>
       </c>
       <c r="U36">
         <f t="shared" si="3"/>
-        <v>0.20420150399273782</v>
+        <v>0.24077490769292967</v>
       </c>
       <c r="V36">
         <f t="shared" si="4"/>
-        <v>61.467889908256879</v>
+        <v>72.477064220183479</v>
       </c>
       <c r="W36">
         <f>V36*L36/1000</f>
-        <v>14.532765402296022</v>
+        <v>17.135648757931129</v>
       </c>
       <c r="X36">
         <f>C36*V36/1000</f>
-        <v>40.937614678899081</v>
+        <v>48.269724770642199</v>
       </c>
     </row>
     <row r="37" spans="1:25" ht="13.15" x14ac:dyDescent="0.4">
@@ -3213,7 +3214,7 @@
         <v>430.46449643717398</v>
       </c>
       <c r="O40" s="41">
-        <v>6.5</v>
+        <v>4.8</v>
       </c>
       <c r="P40" s="42">
         <v>1090730141</v>
@@ -3231,19 +3232,19 @@
       </c>
       <c r="T40">
         <f t="shared" si="2"/>
-        <v>1.9420017385064384E-2</v>
+        <v>2.6923205920202888E-2</v>
       </c>
       <c r="U40">
         <f t="shared" si="3"/>
-        <v>3.7009128985887464E-2</v>
+        <v>5.1308110639525797E-2</v>
       </c>
       <c r="V40">
         <f t="shared" si="4"/>
-        <v>40.366972477064223</v>
+        <v>55.963302752293572</v>
       </c>
       <c r="Y40">
         <f>H40*V40/1000</f>
-        <v>1.438126396704134</v>
+        <v>1.9937661408852765</v>
       </c>
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3287,15 +3288,15 @@
       <c r="N44" s="57"/>
       <c r="T44">
         <f>MAX(T3:T5,T12,T13,T14,T21,T22,T23,T30,T31,T32,T39)</f>
-        <v>0.57031800320803872</v>
+        <v>0.5227915029407022</v>
       </c>
       <c r="U44">
         <f t="shared" ref="U44:V44" si="5">MAX(U3:U5,U12,U13,U14,U21,U22,U23,U30,U31,U32,U39)</f>
-        <v>0.96211564590387966</v>
+        <v>0.88193934207855629</v>
       </c>
       <c r="V44">
         <f t="shared" si="5"/>
-        <v>84.403669724770651</v>
+        <v>70.642201834862391</v>
       </c>
       <c r="W44">
         <f>MAX(W3:W40)</f>
@@ -3303,11 +3304,11 @@
       </c>
       <c r="X44">
         <f t="shared" ref="X44:Y44" si="6">MAX(X3:X40)</f>
-        <v>92.753211009174308</v>
+        <v>75.425688073394497</v>
       </c>
       <c r="Y44">
         <f t="shared" si="6"/>
-        <v>17.292104806954921</v>
+        <v>16.409918880803648</v>
       </c>
     </row>
     <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3402,7 +3403,7 @@
       </c>
       <c r="U46">
         <f t="shared" ref="U46:V46" si="8">MAX(U7:U9,U16,U17,U18,U25,U26,U27,U34,U35,U36,U40)</f>
-        <v>0.22235733287249995</v>
+        <v>0.24687047497629494</v>
       </c>
       <c r="V46">
         <f t="shared" si="8"/>

</xml_diff>